<commit_message>
updated example data per email from bjorn and tests passing
</commit_message>
<xml_diff>
--- a/data/Composition Example Model Changed.xlsx
+++ b/data/Composition Example Model Changed.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\ricks-cafe-american\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Composition" sheetId="1" r:id="rId1"/>
     <sheet name="Composition IDs" sheetId="2" r:id="rId2"/>
+    <sheet name="Renames" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="136">
   <si>
     <t>Component</t>
   </si>
@@ -427,6 +428,12 @@
   </si>
   <si>
     <t>Big Cylinder</t>
+  </si>
+  <si>
+    <t>new name</t>
+  </si>
+  <si>
+    <t>old name</t>
   </si>
 </sst>
 </file>
@@ -1002,9 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1527,4 +1532,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added a function to replace the new names with the corresponding old name from the changed df. Also added a function to determine which column in the rename sheet corresponds to the new names.
</commit_message>
<xml_diff>
--- a/data/Composition Example Model Changed.xlsx
+++ b/data/Composition Example Model Changed.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Composition" sheetId="1" r:id="rId1"/>
     <sheet name="Composition IDs" sheetId="2" r:id="rId2"/>
+    <sheet name="Renames" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="136">
   <si>
     <t>Component</t>
   </si>
@@ -427,6 +428,12 @@
   </si>
   <si>
     <t>Big Cylinder</t>
+  </si>
+  <si>
+    <t>old name</t>
+  </si>
+  <si>
+    <t>new name</t>
   </si>
 </sst>
 </file>
@@ -746,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1002,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1527,4 +1534,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add Composition Example Model Changed.xlsx
</commit_message>
<xml_diff>
--- a/data/Composition Example Model Changed.xlsx
+++ b/data/Composition Example Model Changed.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\ricks-cafe-american\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Composition" sheetId="1" r:id="rId1"/>
     <sheet name="Composition IDs" sheetId="2" r:id="rId2"/>
+    <sheet name="Renames" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="136">
   <si>
     <t>Component</t>
   </si>
@@ -427,6 +428,12 @@
   </si>
   <si>
     <t>Big Cylinder</t>
+  </si>
+  <si>
+    <t>new name</t>
+  </si>
+  <si>
+    <t>old name</t>
   </si>
 </sst>
 </file>
@@ -1002,9 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1527,4 +1532,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>